<commit_message>
Add detection table prototype
</commit_message>
<xml_diff>
--- a/notebooks/data/test.xlsx
+++ b/notebooks/data/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danny\PycharmProjects\documentor\notebooks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0305F7-C8F5-45DD-9C92-04B296E0E18D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C9B8CD-763B-4B5C-A87F-CAC2211BAA04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="20">
   <si>
     <t>A</t>
   </si>
@@ -70,6 +70,21 @@
   </si>
   <si>
     <t>D4</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>E4</t>
   </si>
 </sst>
 </file>
@@ -180,13 +195,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -470,99 +484,153 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5">
-        <v>1</v>
-      </c>
-      <c r="D3" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>1</v>
-      </c>
-      <c r="B4" s="5">
-        <v>1</v>
-      </c>
-      <c r="C4" s="5">
-        <v>1</v>
-      </c>
-      <c r="D4" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>1</v>
-      </c>
-      <c r="B5" s="5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>1</v>
-      </c>
-      <c r="B6" s="5">
-        <v>1</v>
-      </c>
-      <c r="C6" s="5">
-        <v>1</v>
-      </c>
-      <c r="D6" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -576,77 +644,77 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>2</v>
-      </c>
-      <c r="B9" s="2">
-        <v>2</v>
-      </c>
-      <c r="C9" s="2">
-        <v>2</v>
-      </c>
-      <c r="D9" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>2</v>
-      </c>
-      <c r="B10" s="2">
-        <v>2</v>
-      </c>
-      <c r="C10" s="2">
-        <v>2</v>
-      </c>
-      <c r="D10" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>2</v>
-      </c>
-      <c r="B11" s="2">
-        <v>2</v>
-      </c>
-      <c r="C11" s="2">
-        <v>2</v>
-      </c>
-      <c r="D11" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>2</v>
-      </c>
-      <c r="B12" s="2">
-        <v>2</v>
-      </c>
-      <c r="C12" s="2">
-        <v>2</v>
-      </c>
-      <c r="D12" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>2</v>
-      </c>
-      <c r="B13" s="2">
-        <v>2</v>
-      </c>
-      <c r="C13" s="2">
-        <v>2</v>
-      </c>
-      <c r="D13" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="1" t="s">
         <v>8</v>
@@ -658,62 +726,54 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="2">
-        <v>3</v>
-      </c>
-      <c r="C16" s="2">
-        <v>3</v>
-      </c>
-      <c r="D16" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="2">
-        <v>3</v>
-      </c>
-      <c r="C17" s="2">
-        <v>3</v>
-      </c>
-      <c r="D17" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="2">
-        <v>3</v>
-      </c>
-      <c r="C18" s="2">
-        <v>3</v>
-      </c>
-      <c r="D18" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="2">
-        <v>3</v>
-      </c>
-      <c r="C19" s="2">
-        <v>3</v>
-      </c>
-      <c r="D19" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="2">
-        <v>3</v>
-      </c>
-      <c r="C20" s="2">
-        <v>3</v>
-      </c>
-      <c r="D20" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>12</v>
       </c>
@@ -726,55 +786,104 @@
       <c r="E23" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="2">
-        <v>4</v>
-      </c>
-      <c r="C25" s="2">
-        <v>4</v>
+      <c r="E24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="D25" s="2"/>
-      <c r="E25" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="2">
-        <v>4</v>
-      </c>
-      <c r="C26" s="2">
-        <v>4</v>
+      <c r="E25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
+      <c r="F26" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
-      <c r="C28" s="2">
-        <v>4</v>
-      </c>
-      <c r="D28" s="2">
-        <v>4</v>
-      </c>
-      <c r="E28" s="2">
-        <v>4</v>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>